<commit_message>
Latest Code with Test Suite
</commit_message>
<xml_diff>
--- a/Data Files/userdetails.xlsx
+++ b/Data Files/userdetails.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuvaan\git\KatalonLatestDemo\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuvaan\git\KatalonLatestDemo3\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213F3F60-2240-4727-9391-277DD6A45C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B67043-9EFF-44A3-BC82-5A5A76151608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19150" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19150" windowHeight="11260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +41,15 @@
   </si>
   <si>
     <t>siddarth.punamiya@ica.se</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>RyzK/uu8Q18DVx3DwtARbQ==</t>
+  </si>
+  <si>
+    <t>g3/DOGG74jC3Flrr3yH+3D/yKbOqqUNM</t>
   </si>
 </sst>
 </file>
@@ -370,7 +380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -411,4 +421,46 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176F8097-FFF5-47BE-995B-62E5FAC4AA15}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>